<commit_message>
Hand-checked the AUC calculation for inulin no ABX summer samples
</commit_message>
<xml_diff>
--- a/fariba_fortran/Fariba_Inulin_AUC_Calcs.xlsx
+++ b/fariba_fortran/Fariba_Inulin_AUC_Calcs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/CRDS_Calcs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/CRDS_Calcs/fariba_fortran/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="112" documentId="13_ncr:1_{559865C5-51A1-4D4A-8D0A-B573284CE70E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABF52FC9-5D0E-466C-B2A5-2BE2D6653FCB}"/>
+  <xr:revisionPtr revIDLastSave="482" documentId="13_ncr:1_{559865C5-51A1-4D4A-8D0A-B573284CE70E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39640FBD-3B78-4226-BBEC-5864423D973A}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="70">
   <si>
     <t>RelTime</t>
   </si>
@@ -237,6 +237,15 @@
   <si>
     <t>Normalized end time -&gt;</t>
   </si>
+  <si>
+    <t>&lt;- removed</t>
+  </si>
+  <si>
+    <t>Checking calculation with S03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normalized end time = </t>
+  </si>
 </sst>
 </file>
 
@@ -262,7 +271,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -272,6 +281,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -288,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
@@ -300,6 +321,8 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,13 +605,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L639"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="F131" sqref="F131"/>
+    <sheetView tabSelected="1" topLeftCell="A344" workbookViewId="0">
+      <selection activeCell="K379" sqref="K379"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
     <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
@@ -641,7 +665,7 @@
         <v>3</v>
       </c>
       <c r="I3">
-        <f>B3+23.54</f>
+        <f t="shared" ref="I3:I17" si="0">B3+23.54</f>
         <v>0</v>
       </c>
       <c r="J3">
@@ -649,7 +673,7 @@
         <v>97.784999999999997</v>
       </c>
       <c r="K3">
-        <f>A4-A3</f>
+        <f t="shared" ref="K3:K16" si="1">A4-A3</f>
         <v>0.1</v>
       </c>
       <c r="L3">
@@ -668,19 +692,19 @@
         <v>3</v>
       </c>
       <c r="I4">
-        <f>B4+23.54</f>
+        <f t="shared" si="0"/>
         <v>195.57</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J16" si="0">(I5+I4)/2</f>
+        <f t="shared" ref="J4:J13" si="2">(I5+I4)/2</f>
         <v>327.51499999999999</v>
       </c>
       <c r="K4">
-        <f>A5-A4</f>
+        <f t="shared" si="1"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L4:L16" si="1">J4*K4</f>
+        <f t="shared" ref="L4:L13" si="3">J4*K4</f>
         <v>98.254500000000007</v>
       </c>
     </row>
@@ -695,19 +719,19 @@
         <v>3</v>
       </c>
       <c r="I5">
-        <f>B5+23.54</f>
+        <f t="shared" si="0"/>
         <v>459.46000000000004</v>
       </c>
       <c r="J5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>511.89499999999998</v>
       </c>
       <c r="K5">
-        <f>A6-A5</f>
+        <f t="shared" si="1"/>
         <v>0.32999999999999996</v>
       </c>
       <c r="L5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>168.92534999999998</v>
       </c>
     </row>
@@ -722,19 +746,19 @@
         <v>3</v>
       </c>
       <c r="I6">
-        <f>B6+23.54</f>
+        <f t="shared" si="0"/>
         <v>564.32999999999993</v>
       </c>
       <c r="J6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>637.58999999999992</v>
       </c>
       <c r="K6">
-        <f>A7-A6</f>
+        <f t="shared" si="1"/>
         <v>0.29000000000000004</v>
       </c>
       <c r="L6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>184.90109999999999</v>
       </c>
     </row>
@@ -749,19 +773,19 @@
         <v>3</v>
       </c>
       <c r="I7">
-        <f>B7+23.54</f>
+        <f t="shared" si="0"/>
         <v>710.84999999999991</v>
       </c>
       <c r="J7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>948.55499999999995</v>
       </c>
       <c r="K7">
-        <f>A8-A7</f>
+        <f t="shared" si="1"/>
         <v>0.31000000000000005</v>
       </c>
       <c r="L7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>294.05205000000001</v>
       </c>
     </row>
@@ -776,19 +800,19 @@
         <v>3</v>
       </c>
       <c r="I8">
-        <f>B8+23.54</f>
+        <f t="shared" si="0"/>
         <v>1186.26</v>
       </c>
       <c r="J8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1572.24</v>
       </c>
       <c r="K8">
-        <f>A9-A8</f>
+        <f t="shared" si="1"/>
         <v>0.29999999999999982</v>
       </c>
       <c r="L8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>471.67199999999974</v>
       </c>
     </row>
@@ -803,19 +827,19 @@
         <v>3</v>
       </c>
       <c r="I9">
-        <f>B9+23.54</f>
+        <f t="shared" si="0"/>
         <v>1958.22</v>
       </c>
       <c r="J9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2140.0149999999999</v>
       </c>
       <c r="K9">
-        <f>A10-A9</f>
+        <f t="shared" si="1"/>
         <v>0.37000000000000011</v>
       </c>
       <c r="L9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>791.80555000000015</v>
       </c>
     </row>
@@ -830,19 +854,19 @@
         <v>3</v>
       </c>
       <c r="I10">
-        <f>B10+23.54</f>
+        <f t="shared" si="0"/>
         <v>2321.81</v>
       </c>
       <c r="J10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2656.4650000000001</v>
       </c>
       <c r="K10">
-        <f>A11-A10</f>
+        <f t="shared" si="1"/>
         <v>0.31999999999999984</v>
       </c>
       <c r="L10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>850.06879999999967</v>
       </c>
     </row>
@@ -857,19 +881,19 @@
         <v>3</v>
       </c>
       <c r="I11">
-        <f>B11+23.54</f>
+        <f t="shared" si="0"/>
         <v>2991.12</v>
       </c>
       <c r="J11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2928.4700000000003</v>
       </c>
       <c r="K11">
-        <f>A12-A11</f>
+        <f t="shared" si="1"/>
         <v>0.31000000000000005</v>
       </c>
       <c r="L11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>907.82570000000021</v>
       </c>
     </row>
@@ -884,19 +908,19 @@
         <v>3</v>
       </c>
       <c r="I12">
-        <f>B12+23.54</f>
+        <f t="shared" si="0"/>
         <v>2865.82</v>
       </c>
       <c r="J12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3260.04</v>
       </c>
       <c r="K12">
-        <f>A13-A12</f>
+        <f t="shared" si="1"/>
         <v>0.30000000000000027</v>
       </c>
       <c r="L12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>978.01200000000085</v>
       </c>
     </row>
@@ -911,19 +935,19 @@
         <v>3</v>
       </c>
       <c r="I13">
-        <f>B13+23.54</f>
+        <f t="shared" si="0"/>
         <v>3654.2599999999998</v>
       </c>
       <c r="J13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3935.3999999999996</v>
       </c>
       <c r="K13">
-        <f>A14-A13</f>
+        <f t="shared" si="1"/>
         <v>0.31999999999999984</v>
       </c>
       <c r="L13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1259.3279999999993</v>
       </c>
     </row>
@@ -938,7 +962,7 @@
         <v>3</v>
       </c>
       <c r="I14">
-        <f>B14+23.54</f>
+        <f t="shared" si="0"/>
         <v>4216.54</v>
       </c>
       <c r="J14">
@@ -946,7 +970,7 @@
         <v>3195.1099999999997</v>
       </c>
       <c r="K14">
-        <f>A15-A14</f>
+        <f t="shared" si="1"/>
         <v>0.70000000000000018</v>
       </c>
       <c r="L14">
@@ -968,19 +992,19 @@
         <v>64</v>
       </c>
       <c r="I15">
-        <f>B15+23.54</f>
+        <f t="shared" si="0"/>
         <v>2173.6799999999998</v>
       </c>
       <c r="J15">
-        <f t="shared" ref="J15:J16" si="2">(I16+I15)/2</f>
+        <f t="shared" ref="J15:J16" si="4">(I16+I15)/2</f>
         <v>2274.09</v>
       </c>
       <c r="K15">
-        <f>A16-A15</f>
+        <f t="shared" si="1"/>
         <v>0.28000000000000025</v>
       </c>
       <c r="L15">
-        <f t="shared" ref="L15:L16" si="3">J16*K15</f>
+        <f t="shared" ref="L15:L16" si="5">J16*K15</f>
         <v>641.4954000000007</v>
       </c>
     </row>
@@ -995,19 +1019,19 @@
         <v>3</v>
       </c>
       <c r="I16">
-        <f>B16+23.54</f>
+        <f t="shared" si="0"/>
         <v>2374.5</v>
       </c>
       <c r="J16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2291.0550000000003</v>
       </c>
       <c r="K16">
-        <f>A17-A16</f>
+        <f t="shared" si="1"/>
         <v>0.33999999999999986</v>
       </c>
       <c r="L16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -1022,7 +1046,7 @@
         <v>3</v>
       </c>
       <c r="I17">
-        <f>B17+23.54</f>
+        <f t="shared" si="0"/>
         <v>2207.61</v>
       </c>
       <c r="L17">
@@ -2157,7 +2181,7 @@
         <v>10</v>
       </c>
       <c r="H116">
-        <f t="shared" ref="H116:H130" si="4">B116+25.33</f>
+        <f>B116+25.33</f>
         <v>39.53</v>
       </c>
       <c r="I116">
@@ -2169,11 +2193,11 @@
         <v>0.3</v>
       </c>
       <c r="K116">
-        <f t="shared" ref="K116:K129" si="5">I116*J116</f>
+        <f t="shared" ref="K116:K128" si="6">I116*J116</f>
         <v>21.306000000000001</v>
       </c>
       <c r="L116">
-        <f t="shared" ref="L116:L128" si="6">ABS(K116)</f>
+        <f t="shared" ref="L116:L128" si="7">ABS(K116)</f>
         <v>21.306000000000001</v>
       </c>
     </row>
@@ -2188,11 +2212,11 @@
         <v>10</v>
       </c>
       <c r="H117">
-        <f t="shared" si="4"/>
+        <f>B117+25.33</f>
         <v>102.51</v>
       </c>
       <c r="I117">
-        <f t="shared" ref="I117:I119" si="7">(H118+H117)/2</f>
+        <f>(H118+H117)/2</f>
         <v>144.67499999999998</v>
       </c>
       <c r="J117">
@@ -2200,11 +2224,11 @@
         <v>0.26666666700000002</v>
       </c>
       <c r="K117">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>38.580000048224996</v>
       </c>
       <c r="L117">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>38.580000048224996</v>
       </c>
     </row>
@@ -2219,11 +2243,11 @@
         <v>10</v>
       </c>
       <c r="H118">
-        <f t="shared" si="4"/>
+        <f>B118+25.33</f>
         <v>186.83999999999997</v>
       </c>
       <c r="I118">
-        <f t="shared" si="7"/>
+        <f>(H119+H118)/2</f>
         <v>204.5</v>
       </c>
       <c r="J118">
@@ -2231,11 +2255,11 @@
         <v>0.30000000000000004</v>
       </c>
       <c r="K118">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>61.350000000000009</v>
       </c>
       <c r="L118">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>61.350000000000009</v>
       </c>
     </row>
@@ -2266,7 +2290,7 @@
         <v>128.82633326553</v>
       </c>
       <c r="L119">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>128.82633326553</v>
       </c>
     </row>
@@ -2296,11 +2320,11 @@
         <v>0.26666666699999997</v>
       </c>
       <c r="K120">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>46.156000057694996</v>
       </c>
       <c r="L120">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>46.156000057694996</v>
       </c>
     </row>
@@ -2315,11 +2339,11 @@
         <v>10</v>
       </c>
       <c r="H121">
-        <f t="shared" ref="H121:H130" si="8">B122+25.33</f>
+        <f>B122+25.33</f>
         <v>161.51</v>
       </c>
       <c r="I121">
-        <f t="shared" ref="I121:I128" si="9">(H122+H121)/2</f>
+        <f>(H122+H121)/2</f>
         <v>151.095</v>
       </c>
       <c r="J121">
@@ -2327,11 +2351,11 @@
         <v>0.30000000000000004</v>
       </c>
       <c r="K121">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>45.328500000000005</v>
       </c>
       <c r="L121">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>45.328500000000005</v>
       </c>
     </row>
@@ -2346,11 +2370,11 @@
         <v>10</v>
       </c>
       <c r="H122">
-        <f t="shared" si="8"/>
+        <f>B123+25.33</f>
         <v>140.68</v>
       </c>
       <c r="I122">
-        <f t="shared" si="9"/>
+        <f>(H123+H122)/2</f>
         <v>131.5</v>
       </c>
       <c r="J122">
@@ -2358,11 +2382,11 @@
         <v>0.28333333299999985</v>
       </c>
       <c r="K122">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>37.25833328949998</v>
       </c>
       <c r="L122">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>37.25833328949998</v>
       </c>
     </row>
@@ -2377,11 +2401,11 @@
         <v>10</v>
       </c>
       <c r="H123">
-        <f t="shared" si="8"/>
+        <f>B124+25.33</f>
         <v>122.32</v>
       </c>
       <c r="I123">
-        <f t="shared" si="9"/>
+        <f>(H124+H123)/2</f>
         <v>115.82</v>
       </c>
       <c r="J123">
@@ -2389,11 +2413,11 @@
         <v>0.26666666699999997</v>
       </c>
       <c r="K123">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>30.885333371939996</v>
       </c>
       <c r="L123">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>30.885333371939996</v>
       </c>
     </row>
@@ -2408,11 +2432,11 @@
         <v>10</v>
       </c>
       <c r="H124">
-        <f t="shared" si="8"/>
+        <f>B125+25.33</f>
         <v>109.32</v>
       </c>
       <c r="I124">
-        <f t="shared" si="9"/>
+        <f>(H125+H124)/2</f>
         <v>101.74</v>
       </c>
       <c r="J124">
@@ -2420,11 +2444,11 @@
         <v>0.2833333330000003</v>
       </c>
       <c r="K124">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>28.826333299420028</v>
       </c>
       <c r="L124">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>28.826333299420028</v>
       </c>
     </row>
@@ -2439,11 +2463,11 @@
         <v>10</v>
       </c>
       <c r="H125">
-        <f t="shared" si="8"/>
+        <f>B126+25.33</f>
         <v>94.16</v>
       </c>
       <c r="I125">
-        <f t="shared" si="9"/>
+        <f>(H126+H125)/2</f>
         <v>89.435000000000002</v>
       </c>
       <c r="J125">
@@ -2451,11 +2475,11 @@
         <v>0.28333333399999994</v>
       </c>
       <c r="K125">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>25.339916726289996</v>
       </c>
       <c r="L125">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>25.339916726289996</v>
       </c>
     </row>
@@ -2470,11 +2494,11 @@
         <v>10</v>
       </c>
       <c r="H126">
-        <f t="shared" si="8"/>
+        <f>B127+25.33</f>
         <v>84.710000000000008</v>
       </c>
       <c r="I126">
-        <f t="shared" si="9"/>
+        <f>(H127+H126)/2</f>
         <v>81.03</v>
       </c>
       <c r="J126">
@@ -2482,11 +2506,11 @@
         <v>0.29999999999999982</v>
       </c>
       <c r="K126">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>24.308999999999987</v>
       </c>
       <c r="L126">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>24.308999999999987</v>
       </c>
     </row>
@@ -2501,11 +2525,11 @@
         <v>10</v>
       </c>
       <c r="H127">
-        <f t="shared" si="8"/>
+        <f>B128+25.33</f>
         <v>77.349999999999994</v>
       </c>
       <c r="I127">
-        <f t="shared" si="9"/>
+        <f>(H128+H127)/2</f>
         <v>74.3</v>
       </c>
       <c r="J127">
@@ -2513,11 +2537,11 @@
         <v>0.30000000000000027</v>
       </c>
       <c r="K127">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>22.29000000000002</v>
       </c>
       <c r="L127">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>22.29000000000002</v>
       </c>
     </row>
@@ -2532,11 +2556,11 @@
         <v>10</v>
       </c>
       <c r="H128">
-        <f t="shared" si="8"/>
+        <f>B129+25.33</f>
         <v>71.25</v>
       </c>
       <c r="I128">
-        <f t="shared" si="9"/>
+        <f>(H129+H128)/2</f>
         <v>65.314999999999998</v>
       </c>
       <c r="J128">
@@ -2544,11 +2568,11 @@
         <v>0.10000333300000008</v>
       </c>
       <c r="K128">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.5317176948950051</v>
       </c>
       <c r="L128">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.5317176948950051</v>
       </c>
     </row>
@@ -3450,7 +3474,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>3.9166666669999999</v>
       </c>
@@ -3461,7 +3485,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>4.2166666670000001</v>
       </c>
@@ -3472,7 +3496,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>0</v>
       </c>
@@ -3483,7 +3507,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>0.16666666699999999</v>
       </c>
@@ -3494,7 +3518,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>0.45</v>
       </c>
@@ -3505,7 +3529,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>0.78333333299999997</v>
       </c>
@@ -3516,7 +3540,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>1.066666667</v>
       </c>
@@ -3527,7 +3551,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>1.35</v>
       </c>
@@ -3538,7 +3562,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>1.6333333329999999</v>
       </c>
@@ -3549,7 +3573,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>1.9166666670000001</v>
       </c>
@@ -3560,7 +3584,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>2.1666666669999999</v>
       </c>
@@ -3571,7 +3595,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>2.4500000000000002</v>
       </c>
@@ -3582,7 +3606,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>2.733333333</v>
       </c>
@@ -3593,7 +3617,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>3.3833333329999999</v>
       </c>
@@ -3604,7 +3628,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>3.6666666669999999</v>
       </c>
@@ -3615,7 +3639,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>3.9333333330000002</v>
       </c>
@@ -3625,8 +3649,11 @@
       <c r="C224" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H224" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>4.233333333</v>
       </c>
@@ -3636,470 +3663,1082 @@
       <c r="C225" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A226">
+      <c r="H225" t="s">
+        <v>59</v>
+      </c>
+      <c r="I225" t="s">
+        <v>60</v>
+      </c>
+      <c r="J225" t="s">
+        <v>61</v>
+      </c>
+      <c r="K225" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="226" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A226" s="9">
         <v>0</v>
       </c>
-      <c r="B226">
+      <c r="B226" s="9">
         <v>-22.19</v>
       </c>
-      <c r="C226" t="s">
+      <c r="C226" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A227">
+      <c r="H226" s="9">
+        <f>B226+22.19</f>
+        <v>0</v>
+      </c>
+      <c r="I226" s="9">
+        <f>(H227+H226)/2</f>
+        <v>162.52500000000001</v>
+      </c>
+      <c r="J226" s="9">
+        <f>A228-A226</f>
+        <v>0.61666666699999995</v>
+      </c>
+      <c r="K226" s="9">
+        <f>I226*J226</f>
+        <v>100.223750054175</v>
+      </c>
+    </row>
+    <row r="227" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A227" s="9">
         <v>0.233333333</v>
       </c>
-      <c r="B227">
+      <c r="B227" s="9">
         <v>201.19</v>
       </c>
-      <c r="C227" t="s">
+      <c r="C227" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A228">
+      <c r="D227" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H227" s="9">
+        <f>B228+22.19</f>
+        <v>325.05</v>
+      </c>
+      <c r="I227" s="9">
+        <f>(H228+H227)/2</f>
+        <v>312.90499999999997</v>
+      </c>
+      <c r="J227" s="9">
+        <f>A229-A228</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="K227" s="9">
+        <f>I227*J227</f>
+        <v>93.871500000000012</v>
+      </c>
+    </row>
+    <row r="228" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A228" s="9">
         <v>0.61666666699999995</v>
       </c>
-      <c r="B228">
+      <c r="B228" s="9">
         <v>302.86</v>
       </c>
-      <c r="C228" t="s">
+      <c r="C228" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A229">
+      <c r="H228" s="9">
+        <f>B229+22.19</f>
+        <v>300.76</v>
+      </c>
+      <c r="I228" s="9">
+        <f>(H229+H228)/2</f>
+        <v>279.96500000000003</v>
+      </c>
+      <c r="J228" s="9">
+        <f>A230-A229</f>
+        <v>0.29999999999999993</v>
+      </c>
+      <c r="K228" s="9">
+        <f>I228*J228</f>
+        <v>83.989499999999992</v>
+      </c>
+    </row>
+    <row r="229" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A229" s="9">
         <v>0.91666666699999999</v>
       </c>
-      <c r="B229">
+      <c r="B229" s="9">
         <v>278.57</v>
       </c>
-      <c r="C229" t="s">
+      <c r="C229" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A230">
+      <c r="H229" s="9">
+        <f>B230+22.19</f>
+        <v>259.17</v>
+      </c>
+      <c r="I229" s="9">
+        <f>(H230+H229)/2</f>
+        <v>235.62</v>
+      </c>
+      <c r="J229" s="9">
+        <f>A231-A230</f>
+        <v>0.31666666600000015</v>
+      </c>
+      <c r="K229" s="9">
+        <f>I229*J229</f>
+        <v>74.612999842920033</v>
+      </c>
+    </row>
+    <row r="230" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A230" s="9">
         <v>1.2166666669999999</v>
       </c>
-      <c r="B230">
+      <c r="B230" s="9">
         <v>236.98</v>
       </c>
-      <c r="C230" t="s">
+      <c r="C230" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A231">
+      <c r="H230" s="9">
+        <f>B231+22.19</f>
+        <v>212.07</v>
+      </c>
+      <c r="I230" s="9">
+        <f>(H231+H230)/2</f>
+        <v>196.64999999999998</v>
+      </c>
+      <c r="J230" s="9">
+        <f>A232-A231</f>
+        <v>0.31666666700000001</v>
+      </c>
+      <c r="K230" s="9">
+        <f>I230*J230</f>
+        <v>62.272500065549998</v>
+      </c>
+    </row>
+    <row r="231" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A231" s="9">
         <v>1.5333333330000001</v>
       </c>
-      <c r="B231">
+      <c r="B231" s="9">
         <v>189.88</v>
       </c>
-      <c r="C231" t="s">
+      <c r="C231" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A232">
+      <c r="H231" s="9">
+        <f>B232+22.19</f>
+        <v>181.23</v>
+      </c>
+      <c r="I231" s="9">
+        <f>(H232+H231)/2</f>
+        <v>303.59999999999997</v>
+      </c>
+      <c r="J231" s="9">
+        <f>A234-A232</f>
+        <v>0.68333333299999977</v>
+      </c>
+      <c r="K231" s="9">
+        <f>I231*J231</f>
+        <v>207.45999989879991</v>
+      </c>
+    </row>
+    <row r="232" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A232" s="9">
         <v>1.85</v>
       </c>
-      <c r="B232">
+      <c r="B232" s="9">
         <v>159.04</v>
       </c>
-      <c r="C232" t="s">
+      <c r="C232" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A233">
+      <c r="H232" s="9">
+        <f>B234+22.19</f>
+        <v>425.96999999999997</v>
+      </c>
+      <c r="I232" s="9">
+        <f>(H233+H232)/2</f>
+        <v>925.43000000000006</v>
+      </c>
+      <c r="J232" s="9">
+        <f>A235-A234</f>
+        <v>0.26666666699999997</v>
+      </c>
+      <c r="K232" s="9">
+        <f>I232*J232</f>
+        <v>246.78133364180999</v>
+      </c>
+    </row>
+    <row r="233" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A233" s="9">
         <v>2.1666666669999999</v>
       </c>
-      <c r="B233">
+      <c r="B233" s="9">
         <v>118.02</v>
       </c>
-      <c r="C233" t="s">
+      <c r="C233" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A234">
+      <c r="D233" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H233" s="9">
+        <f>B235+22.19</f>
+        <v>1424.89</v>
+      </c>
+      <c r="I233" s="9">
+        <f>(H234+H233)/2</f>
+        <v>1789.63</v>
+      </c>
+      <c r="J233" s="9">
+        <f>A236-A235</f>
+        <v>0.36666666700000006</v>
+      </c>
+      <c r="K233" s="9">
+        <f>I233*J233</f>
+        <v>656.19766726321018</v>
+      </c>
+    </row>
+    <row r="234" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A234" s="9">
         <v>2.5333333329999999</v>
       </c>
-      <c r="B234">
+      <c r="B234" s="9">
         <v>403.78</v>
       </c>
-      <c r="C234" t="s">
+      <c r="C234" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A235">
+      <c r="H234" s="9">
+        <f>B236+22.19</f>
+        <v>2154.37</v>
+      </c>
+      <c r="I234" s="9">
+        <f>(H235+H234)/2</f>
+        <v>2346.2449999999999</v>
+      </c>
+      <c r="J234" s="9">
+        <f>A237-A236</f>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="K234" s="9">
+        <f>I234*J234</f>
+        <v>821.18575000000021</v>
+      </c>
+    </row>
+    <row r="235" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A235" s="9">
         <v>2.8</v>
       </c>
-      <c r="B235">
+      <c r="B235" s="9">
         <v>1402.7</v>
       </c>
-      <c r="C235" t="s">
+      <c r="C235" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A236">
+      <c r="H235" s="9">
+        <f>B237+22.19</f>
+        <v>2538.12</v>
+      </c>
+      <c r="I235" s="9">
+        <f>(H236+H235)/2</f>
+        <v>2590.105</v>
+      </c>
+      <c r="J235" s="9">
+        <f>A238-A237</f>
+        <v>0.31666666600000015</v>
+      </c>
+      <c r="K235" s="9">
+        <f>I235*J235</f>
+        <v>820.19991493993041</v>
+      </c>
+    </row>
+    <row r="236" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A236" s="9">
         <v>3.1666666669999999</v>
       </c>
-      <c r="B236">
+      <c r="B236" s="9">
         <v>2132.1799999999998</v>
       </c>
-      <c r="C236" t="s">
+      <c r="C236" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A237">
+      <c r="H236" s="9">
+        <f>B238+22.19</f>
+        <v>2642.09</v>
+      </c>
+      <c r="I236" s="9">
+        <f>(H237+H236)/2</f>
+        <v>2543.5349999999999</v>
+      </c>
+      <c r="J236" s="9">
+        <f>G237-A238</f>
+        <v>0.23333666700000011</v>
+      </c>
+      <c r="K236" s="9">
+        <f>I236*J236</f>
+        <v>593.49997929784524</v>
+      </c>
+    </row>
+    <row r="237" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A237" s="9">
         <v>3.516666667</v>
       </c>
-      <c r="B237">
+      <c r="B237" s="9">
         <v>2515.9299999999998</v>
       </c>
-      <c r="C237" t="s">
+      <c r="C237" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A238">
+      <c r="E237" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G237">
+        <v>4.0666700000000002</v>
+      </c>
+      <c r="H237" s="9">
+        <f>B239+22.19</f>
+        <v>2444.98</v>
+      </c>
+      <c r="K237" s="9">
+        <f>SUM(K226:K236)</f>
+        <v>3760.2948950042405</v>
+      </c>
+    </row>
+    <row r="238" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A238" s="9">
         <v>3.8333333330000001</v>
       </c>
-      <c r="B238">
+      <c r="B238" s="9">
         <v>2619.9</v>
       </c>
-      <c r="C238" t="s">
+      <c r="C238" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A239">
+    <row r="239" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A239" s="9">
         <v>4.1666666670000003</v>
       </c>
-      <c r="B239">
+      <c r="B239" s="9">
         <v>2422.79</v>
       </c>
-      <c r="C239" t="s">
+      <c r="C239" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A240">
+      <c r="H239" t="s">
+        <v>59</v>
+      </c>
+      <c r="I239" t="s">
+        <v>60</v>
+      </c>
+      <c r="J239" t="s">
+        <v>61</v>
+      </c>
+      <c r="K239" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="240" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A240" s="10">
         <v>0</v>
       </c>
-      <c r="B240">
+      <c r="B240" s="10">
         <v>-19.21</v>
       </c>
-      <c r="C240" t="s">
+      <c r="C240" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A241">
+      <c r="H240" s="10">
+        <f>B240+19.21</f>
+        <v>0</v>
+      </c>
+      <c r="I240" s="10">
+        <f>(H241+H240)/2</f>
+        <v>30.734999999999999</v>
+      </c>
+      <c r="J240" s="10">
+        <f>A241-A240</f>
         <v>0.16666666699999999</v>
       </c>
-      <c r="B241">
+      <c r="K240" s="10">
+        <f>I240*J240</f>
+        <v>5.122500010245</v>
+      </c>
+    </row>
+    <row r="241" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A241" s="10">
+        <v>0.16666666699999999</v>
+      </c>
+      <c r="B241" s="10">
         <v>42.26</v>
       </c>
-      <c r="C241" t="s">
+      <c r="C241" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A242">
+      <c r="H241" s="10">
+        <f>B241+19.21</f>
+        <v>61.47</v>
+      </c>
+      <c r="I241" s="10">
+        <f>(H242+H241)/2</f>
+        <v>112.905</v>
+      </c>
+      <c r="J241" s="10">
+        <f>A243-A241</f>
+        <v>0.7</v>
+      </c>
+      <c r="K241" s="10">
+        <f>I241*J241</f>
+        <v>79.033499999999989</v>
+      </c>
+    </row>
+    <row r="242" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A242" s="10">
         <v>0.5</v>
       </c>
-      <c r="B242">
+      <c r="B242" s="10">
         <v>1272.5</v>
       </c>
-      <c r="C242" t="s">
+      <c r="C242" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A243">
+      <c r="D242" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="H242" s="10">
+        <f>B243+19.21</f>
+        <v>164.34</v>
+      </c>
+      <c r="I242" s="10">
+        <f>(H243+H242)/2</f>
+        <v>188.02500000000001</v>
+      </c>
+      <c r="J242" s="10">
+        <f>A244-A243</f>
+        <v>0.33333333300000001</v>
+      </c>
+      <c r="K242" s="10">
+        <f>I242*J242</f>
+        <v>62.674999937325005</v>
+      </c>
+    </row>
+    <row r="243" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A243" s="10">
         <v>0.86666666699999995</v>
       </c>
-      <c r="B243">
+      <c r="B243" s="10">
         <v>145.13</v>
       </c>
-      <c r="C243" t="s">
+      <c r="C243" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A244">
+      <c r="H243" s="10">
+        <f t="shared" ref="H243:H244" si="8">B244+19.21</f>
+        <v>211.71</v>
+      </c>
+      <c r="I243" s="10">
+        <f>(H244+H243)/2</f>
+        <v>204.08</v>
+      </c>
+      <c r="J243" s="10">
+        <f t="shared" ref="J243:J247" si="9">A245-A244</f>
+        <v>0.31666666700000001</v>
+      </c>
+      <c r="K243" s="10">
+        <f>I243*J243</f>
+        <v>64.62533340136001</v>
+      </c>
+    </row>
+    <row r="244" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A244" s="10">
         <v>1.2</v>
       </c>
-      <c r="B244">
+      <c r="B244" s="10">
         <v>192.5</v>
       </c>
-      <c r="C244" t="s">
+      <c r="C244" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A245">
+      <c r="H244" s="10">
+        <f t="shared" si="8"/>
+        <v>196.45000000000002</v>
+      </c>
+      <c r="I244" s="10">
+        <f>(H245+H244)/2</f>
+        <v>248.26</v>
+      </c>
+      <c r="J244" s="10">
+        <f>A247-A245</f>
+        <v>0.73333333300000003</v>
+      </c>
+      <c r="K244" s="10">
+        <f>I244*J244</f>
+        <v>182.05733325058</v>
+      </c>
+    </row>
+    <row r="245" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A245" s="10">
         <v>1.516666667</v>
       </c>
-      <c r="B245">
+      <c r="B245" s="10">
         <v>177.24</v>
       </c>
-      <c r="C245" t="s">
+      <c r="C245" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A246">
+      <c r="H245" s="10">
+        <f>B247+19.21</f>
+        <v>300.07</v>
+      </c>
+      <c r="I245" s="10">
+        <f>(H246+H245)/2</f>
+        <v>478.54499999999996</v>
+      </c>
+      <c r="J245" s="10">
+        <f>A248-A247</f>
+        <v>0.33333333300000012</v>
+      </c>
+      <c r="K245" s="10">
+        <f>I245*J245</f>
+        <v>159.51499984048505</v>
+      </c>
+    </row>
+    <row r="246" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A246" s="10">
         <v>1.85</v>
       </c>
-      <c r="B246">
+      <c r="B246" s="10">
         <v>156.77000000000001</v>
       </c>
-      <c r="C246" t="s">
+      <c r="C246" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A247">
+      <c r="D246" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="H246" s="10">
+        <f t="shared" ref="H246:H250" si="10">B248+19.21</f>
+        <v>657.02</v>
+      </c>
+      <c r="I246" s="10">
+        <f>(H247+H246)/2</f>
+        <v>791.95</v>
+      </c>
+      <c r="J246" s="10">
+        <f>A249-A248</f>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="K246" s="10">
+        <f>I246*J246</f>
+        <v>277.18250000000006</v>
+      </c>
+    </row>
+    <row r="247" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A247" s="10">
         <v>2.25</v>
       </c>
-      <c r="B247">
+      <c r="B247" s="10">
         <v>280.86</v>
       </c>
-      <c r="C247" t="s">
+      <c r="C247" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A248">
+      <c r="H247" s="10">
+        <f t="shared" si="10"/>
+        <v>926.88</v>
+      </c>
+      <c r="I247" s="10">
+        <f>(H248+H247)/2</f>
+        <v>999.69499999999994</v>
+      </c>
+      <c r="J247" s="10">
+        <f>A250-A249</f>
+        <v>0.34999999999999964</v>
+      </c>
+      <c r="K247" s="10">
+        <f>I247*J247</f>
+        <v>349.89324999999963</v>
+      </c>
+    </row>
+    <row r="248" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A248" s="10">
         <v>2.5833333330000001</v>
       </c>
-      <c r="B248">
+      <c r="B248" s="10">
         <v>637.80999999999995</v>
       </c>
-      <c r="C248" t="s">
+      <c r="C248" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A249">
+      <c r="H248" s="10">
+        <f t="shared" si="10"/>
+        <v>1072.51</v>
+      </c>
+      <c r="I248" s="10">
+        <f>(H249+H248)/2</f>
+        <v>1034.57</v>
+      </c>
+      <c r="J248" s="10">
+        <f>A251-A250</f>
+        <v>0.3333333340000002</v>
+      </c>
+      <c r="K248" s="10">
+        <f>I248*J248</f>
+        <v>344.85666735638017</v>
+      </c>
+    </row>
+    <row r="249" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A249" s="10">
         <v>2.9333333330000002</v>
       </c>
-      <c r="B249">
+      <c r="B249" s="10">
         <v>907.67</v>
       </c>
-      <c r="C249" t="s">
+      <c r="C249" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A250">
+      <c r="H249" s="10">
+        <f t="shared" si="10"/>
+        <v>996.63</v>
+      </c>
+      <c r="I249" s="10">
+        <f>(H250+H249)/2</f>
+        <v>1012.325</v>
+      </c>
+      <c r="J249" s="10">
+        <f>A252-A251</f>
+        <v>0.29999999999999982</v>
+      </c>
+      <c r="K249" s="10">
+        <f>I249*J249</f>
+        <v>303.69749999999982</v>
+      </c>
+    </row>
+    <row r="250" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A250" s="10">
         <v>3.2833333329999999</v>
       </c>
-      <c r="B250">
+      <c r="B250" s="10">
         <v>1053.3</v>
       </c>
-      <c r="C250" t="s">
+      <c r="C250" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A251">
+      <c r="H250" s="10">
+        <f>B252+19.21</f>
+        <v>1028.02</v>
+      </c>
+      <c r="I250" s="10">
+        <f>(H251+H250)/2</f>
+        <v>1148.0999999999999</v>
+      </c>
+      <c r="J250" s="10">
+        <f>G251-A252</f>
+        <v>0.15000333300000035</v>
+      </c>
+      <c r="K250" s="10">
+        <f>I250*J250</f>
+        <v>172.21882661730038</v>
+      </c>
+    </row>
+    <row r="251" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A251" s="10">
         <v>3.6166666670000001</v>
       </c>
-      <c r="B251">
+      <c r="B251" s="10">
         <v>977.42</v>
       </c>
-      <c r="C251" t="s">
+      <c r="C251" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A252">
+      <c r="E251" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F251" s="9"/>
+      <c r="G251">
+        <v>4.0666700000000002</v>
+      </c>
+      <c r="H251" s="10">
+        <f>B253+19.21</f>
+        <v>1268.18</v>
+      </c>
+      <c r="K251" s="10">
+        <f>SUM(K240:K250)</f>
+        <v>2000.8774104136753</v>
+      </c>
+    </row>
+    <row r="252" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A252" s="10">
         <v>3.9166666669999999</v>
       </c>
-      <c r="B252">
+      <c r="B252" s="10">
         <v>1008.81</v>
       </c>
-      <c r="C252" t="s">
+      <c r="C252" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A253">
+    <row r="253" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A253" s="10">
         <v>4.2166666670000001</v>
       </c>
-      <c r="B253">
+      <c r="B253" s="10">
         <v>1248.97</v>
       </c>
-      <c r="C253" t="s">
+      <c r="C253" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A254">
+      <c r="H253" t="s">
+        <v>59</v>
+      </c>
+      <c r="I253" t="s">
+        <v>60</v>
+      </c>
+      <c r="J253" t="s">
+        <v>61</v>
+      </c>
+      <c r="K253" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="254" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A254" s="9">
         <v>0</v>
       </c>
-      <c r="B254">
+      <c r="B254" s="9">
         <v>-18.95</v>
       </c>
-      <c r="C254" t="s">
+      <c r="C254" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A255">
+      <c r="H254" s="9">
+        <f>B254+18.95</f>
+        <v>0</v>
+      </c>
+      <c r="I254" s="9">
+        <f>(H254+H255)/2</f>
+        <v>-3.0000000000001137E-2</v>
+      </c>
+      <c r="J254" s="9">
+        <f>A255-A254</f>
         <v>0.15</v>
       </c>
-      <c r="B255">
+      <c r="K254" s="9">
+        <f>J254*I254</f>
+        <v>-4.5000000000001705E-3</v>
+      </c>
+    </row>
+    <row r="255" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A255" s="9">
+        <v>0.15</v>
+      </c>
+      <c r="B255" s="9">
         <v>-19.010000000000002</v>
       </c>
-      <c r="C255" t="s">
+      <c r="C255" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A256">
+      <c r="H255" s="9">
+        <f>B255+18.95</f>
+        <v>-6.0000000000002274E-2</v>
+      </c>
+      <c r="I255" s="9">
+        <f t="shared" ref="I255:I263" si="11">(H255+H256)/2</f>
+        <v>180.64499999999998</v>
+      </c>
+      <c r="J255" s="9">
+        <f>A256-A255</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="K255" s="9">
+        <f t="shared" ref="K255:K263" si="12">J255*I255</f>
+        <v>54.1935</v>
+      </c>
+    </row>
+    <row r="256" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A256" s="9">
         <v>0.45</v>
       </c>
-      <c r="B256">
+      <c r="B256" s="9">
         <v>342.4</v>
       </c>
-      <c r="C256" t="s">
+      <c r="C256" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A257">
+      <c r="H256" s="9">
+        <f>B256+18.95</f>
+        <v>361.34999999999997</v>
+      </c>
+      <c r="I256" s="9">
+        <f t="shared" si="11"/>
+        <v>341.46999999999997</v>
+      </c>
+      <c r="J256" s="9">
+        <f>A258-A256</f>
+        <v>0.73333333300000003</v>
+      </c>
+      <c r="K256" s="9">
+        <f t="shared" si="12"/>
+        <v>250.41133321951</v>
+      </c>
+    </row>
+    <row r="257" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A257" s="9">
         <v>0.75</v>
       </c>
-      <c r="B257">
+      <c r="B257" s="9">
         <v>442.78</v>
       </c>
-      <c r="C257" t="s">
+      <c r="C257" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A258">
+      <c r="D257" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H257" s="9">
+        <f>B258+18.95</f>
+        <v>321.58999999999997</v>
+      </c>
+      <c r="I257" s="9">
+        <f t="shared" si="11"/>
+        <v>274.45999999999998</v>
+      </c>
+      <c r="J257" s="9">
+        <f>A259-A258</f>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="K257" s="9">
+        <f t="shared" si="12"/>
+        <v>96.061000000000021</v>
+      </c>
+    </row>
+    <row r="258" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A258" s="9">
         <v>1.183333333</v>
       </c>
-      <c r="B258">
+      <c r="B258" s="9">
         <v>302.64</v>
       </c>
-      <c r="C258" t="s">
+      <c r="C258" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A259">
+      <c r="H258" s="9">
+        <f>B259+18.95</f>
+        <v>227.32999999999998</v>
+      </c>
+      <c r="I258" s="9">
+        <f t="shared" si="11"/>
+        <v>750.19499999999994</v>
+      </c>
+      <c r="J258" s="9">
+        <f>A262-A259</f>
+        <v>1.2</v>
+      </c>
+      <c r="K258" s="9">
+        <f t="shared" si="12"/>
+        <v>900.23399999999992</v>
+      </c>
+    </row>
+    <row r="259" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A259" s="9">
         <v>1.5333333330000001</v>
       </c>
-      <c r="B259">
+      <c r="B259" s="9">
         <v>208.38</v>
       </c>
-      <c r="C259" t="s">
+      <c r="C259" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A260">
+      <c r="H259" s="9">
+        <f>B262+18.95</f>
+        <v>1273.06</v>
+      </c>
+      <c r="I259" s="9">
+        <f t="shared" si="11"/>
+        <v>1695.2499999999998</v>
+      </c>
+      <c r="J259" s="9">
+        <f>A263-A262</f>
+        <v>0.29999999999999982</v>
+      </c>
+      <c r="K259" s="9">
+        <f t="shared" si="12"/>
+        <v>508.57499999999965</v>
+      </c>
+    </row>
+    <row r="260" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A260" s="9">
         <v>1.9</v>
       </c>
-      <c r="B260">
+      <c r="B260" s="9">
         <v>315.8</v>
       </c>
-      <c r="C260" t="s">
+      <c r="C260" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A261">
+      <c r="D260" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H260" s="9">
+        <f>B263+18.95</f>
+        <v>2117.4399999999996</v>
+      </c>
+      <c r="I260" s="9">
+        <f t="shared" si="11"/>
+        <v>2007.4449999999997</v>
+      </c>
+      <c r="J260" s="9">
+        <f>A264-A263</f>
+        <v>0.38333333400000003</v>
+      </c>
+      <c r="K260" s="9">
+        <f t="shared" si="12"/>
+        <v>769.52058467162999</v>
+      </c>
+    </row>
+    <row r="261" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A261" s="9">
         <v>2.3333333330000001</v>
       </c>
-      <c r="B261">
+      <c r="B261" s="9">
         <v>993.45</v>
       </c>
-      <c r="C261" t="s">
+      <c r="C261" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A262">
+      <c r="D261" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H261" s="9">
+        <f>B264+18.95</f>
+        <v>1897.45</v>
+      </c>
+      <c r="I261" s="9">
+        <f t="shared" si="11"/>
+        <v>1947.4650000000001</v>
+      </c>
+      <c r="J261" s="9">
+        <f>A265-A264</f>
+        <v>0.33333333300000012</v>
+      </c>
+      <c r="K261" s="9">
+        <f t="shared" si="12"/>
+        <v>649.15499935084529</v>
+      </c>
+    </row>
+    <row r="262" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A262" s="9">
         <v>2.733333333</v>
       </c>
-      <c r="B262">
+      <c r="B262" s="9">
         <v>1254.1099999999999</v>
       </c>
-      <c r="C262" t="s">
+      <c r="C262" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A263">
+      <c r="H262" s="9">
+        <f>B265+18.95</f>
+        <v>1997.48</v>
+      </c>
+      <c r="I262" s="9">
+        <f t="shared" si="11"/>
+        <v>1946.85</v>
+      </c>
+      <c r="J262" s="9">
+        <f>G264-A265</f>
+        <v>0.31667000000000023</v>
+      </c>
+      <c r="K262" s="9">
+        <f t="shared" si="12"/>
+        <v>616.50898950000044</v>
+      </c>
+    </row>
+    <row r="263" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A263" s="9">
         <v>3.0333333329999999</v>
       </c>
-      <c r="B263">
+      <c r="B263" s="9">
         <v>2098.4899999999998</v>
       </c>
-      <c r="C263" t="s">
+      <c r="C263" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A264">
+      <c r="H263" s="9">
+        <f>B266+18.95</f>
+        <v>1896.22</v>
+      </c>
+      <c r="I263" s="9">
+        <f t="shared" si="11"/>
+        <v>1801.1</v>
+      </c>
+      <c r="J263" s="9">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="K263" s="9">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A264" s="9">
         <v>3.4166666669999999</v>
       </c>
-      <c r="B264">
+      <c r="B264" s="9">
         <v>1878.5</v>
       </c>
-      <c r="C264" t="s">
+      <c r="C264" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A265">
+      <c r="E264" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G264">
+        <v>4.0666700000000002</v>
+      </c>
+      <c r="H264" s="9">
+        <f>B267+18.95</f>
+        <v>1705.98</v>
+      </c>
+      <c r="K264" s="9">
+        <f>SUM(K254:K262)</f>
+        <v>3844.6549067419851</v>
+      </c>
+    </row>
+    <row r="265" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A265" s="9">
         <v>3.75</v>
       </c>
-      <c r="B265">
+      <c r="B265" s="9">
         <v>1978.53</v>
       </c>
-      <c r="C265" t="s">
+      <c r="C265" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A266">
+    <row r="266" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A266" s="9">
         <v>4.1166666669999996</v>
       </c>
-      <c r="B266">
+      <c r="B266" s="9">
         <v>1877.27</v>
       </c>
-      <c r="C266" t="s">
+      <c r="C266" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A267">
+    <row r="267" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A267" s="9">
         <v>4.4333333330000002</v>
       </c>
-      <c r="B267">
+      <c r="B267" s="9">
         <v>1687.03</v>
       </c>
-      <c r="C267" t="s">
+      <c r="C267" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>0</v>
       </c>
@@ -4110,7 +4749,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>0.16666666699999999</v>
       </c>
@@ -4121,7 +4760,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>0.55000000000000004</v>
       </c>
@@ -4132,7 +4771,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>0.88333333300000005</v>
       </c>
@@ -4143,7 +4782,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>1.25</v>
       </c>
@@ -4330,7 +4969,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>3.15</v>
       </c>
@@ -4341,7 +4980,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>4.25</v>
       </c>
@@ -4351,169 +4990,394 @@
       <c r="C290" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A291">
+      <c r="H290" t="s">
+        <v>59</v>
+      </c>
+      <c r="I290" t="s">
+        <v>60</v>
+      </c>
+      <c r="J290" t="s">
+        <v>61</v>
+      </c>
+      <c r="K290" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="291" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A291" s="10">
         <v>0</v>
       </c>
-      <c r="B291">
+      <c r="B291" s="10">
         <v>-20.399999999999999</v>
       </c>
-      <c r="C291" t="s">
+      <c r="C291" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A292">
+      <c r="H291" s="10">
+        <f>B291+20.4</f>
+        <v>0</v>
+      </c>
+      <c r="I291" s="10">
+        <f>(H292+H291)/2</f>
+        <v>153.66999999999999</v>
+      </c>
+      <c r="J291" s="10">
+        <f>A293-A291</f>
+        <v>0.65</v>
+      </c>
+      <c r="K291" s="10">
+        <f>I291*J291</f>
+        <v>99.885499999999993</v>
+      </c>
+    </row>
+    <row r="292" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A292" s="10">
         <v>0.3</v>
       </c>
-      <c r="B292">
+      <c r="B292" s="10">
         <v>173.88</v>
       </c>
-      <c r="C292" t="s">
+      <c r="C292" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A293">
+      <c r="D292" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="H292" s="10">
+        <f>B293+20.4</f>
+        <v>307.33999999999997</v>
+      </c>
+      <c r="I292" s="10">
+        <f t="shared" ref="I292:I302" si="13">(H293+H292)/2</f>
+        <v>352.86500000000001</v>
+      </c>
+      <c r="J292" s="10">
+        <f>A294-A293</f>
+        <v>0.29999999999999993</v>
+      </c>
+      <c r="K292" s="10">
+        <f t="shared" ref="K292:K302" si="14">I292*J292</f>
+        <v>105.85949999999998</v>
+      </c>
+    </row>
+    <row r="293" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A293" s="10">
         <v>0.65</v>
       </c>
-      <c r="B293">
+      <c r="B293" s="10">
         <v>286.94</v>
       </c>
-      <c r="C293" t="s">
+      <c r="C293" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A294">
+      <c r="H293" s="10">
+        <f t="shared" ref="H293:H295" si="15">B294+20.4</f>
+        <v>398.39</v>
+      </c>
+      <c r="I293" s="10">
+        <f t="shared" si="13"/>
+        <v>400.67999999999995</v>
+      </c>
+      <c r="J293" s="10">
+        <f>A295-A294</f>
+        <v>0.31666666700000001</v>
+      </c>
+      <c r="K293" s="10">
+        <f t="shared" si="14"/>
+        <v>126.88200013355998</v>
+      </c>
+    </row>
+    <row r="294" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A294" s="10">
         <v>0.95</v>
       </c>
-      <c r="B294">
+      <c r="B294" s="10">
         <v>377.99</v>
       </c>
-      <c r="C294" t="s">
+      <c r="C294" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A295">
+      <c r="H294" s="10">
+        <f t="shared" si="15"/>
+        <v>402.96999999999997</v>
+      </c>
+      <c r="I294" s="10">
+        <f t="shared" si="13"/>
+        <v>352.41499999999996</v>
+      </c>
+      <c r="J294" s="10">
+        <f>A296-A295</f>
+        <v>0.31666666599999993</v>
+      </c>
+      <c r="K294" s="10">
+        <f t="shared" si="14"/>
+        <v>111.59808309838996</v>
+      </c>
+    </row>
+    <row r="295" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A295" s="10">
         <v>1.266666667</v>
       </c>
-      <c r="B295">
+      <c r="B295" s="10">
         <v>382.57</v>
       </c>
-      <c r="C295" t="s">
+      <c r="C295" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A296">
+      <c r="H295" s="10">
+        <f>B296+20.4</f>
+        <v>301.85999999999996</v>
+      </c>
+      <c r="I295" s="10">
+        <f t="shared" si="13"/>
+        <v>298.15999999999997</v>
+      </c>
+      <c r="J295" s="10">
+        <f>A298-A296</f>
+        <v>0.6666666670000001</v>
+      </c>
+      <c r="K295" s="10">
+        <f t="shared" si="14"/>
+        <v>198.77333343272002</v>
+      </c>
+    </row>
+    <row r="296" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A296" s="10">
         <v>1.5833333329999999</v>
       </c>
-      <c r="B296">
+      <c r="B296" s="10">
         <v>281.45999999999998</v>
       </c>
-      <c r="C296" t="s">
+      <c r="C296" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A297">
+      <c r="H296" s="10">
+        <f>B298+20.4</f>
+        <v>294.45999999999998</v>
+      </c>
+      <c r="I296" s="10">
+        <f t="shared" si="13"/>
+        <v>281.96499999999997</v>
+      </c>
+      <c r="J296" s="10">
+        <f>A299-A298</f>
+        <v>0.33333333300000012</v>
+      </c>
+      <c r="K296" s="10">
+        <f t="shared" si="14"/>
+        <v>93.988333239345025</v>
+      </c>
+    </row>
+    <row r="297" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A297" s="10">
         <v>1.9</v>
       </c>
-      <c r="B297">
+      <c r="B297" s="10">
         <v>292.81</v>
       </c>
-      <c r="C297" t="s">
+      <c r="C297" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A298">
+      <c r="D297" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="H297" s="10">
+        <f t="shared" ref="H297:H300" si="16">B299+20.4</f>
+        <v>269.46999999999997</v>
+      </c>
+      <c r="I297" s="10">
+        <f t="shared" si="13"/>
+        <v>280.27999999999997</v>
+      </c>
+      <c r="J297" s="10">
+        <f>A300-A299</f>
+        <v>0.28333333399999994</v>
+      </c>
+      <c r="K297" s="10">
+        <f t="shared" si="14"/>
+        <v>79.41266685351998</v>
+      </c>
+    </row>
+    <row r="298" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A298" s="10">
         <v>2.25</v>
       </c>
-      <c r="B298">
+      <c r="B298" s="10">
         <v>274.06</v>
       </c>
-      <c r="C298" t="s">
+      <c r="C298" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A299">
+      <c r="H298" s="10">
+        <f t="shared" si="16"/>
+        <v>291.08999999999997</v>
+      </c>
+      <c r="I298" s="10">
+        <f t="shared" si="13"/>
+        <v>526.28499999999997</v>
+      </c>
+      <c r="J298" s="10">
+        <f>A301-A300</f>
+        <v>0.28333333299999985</v>
+      </c>
+      <c r="K298" s="10">
+        <f t="shared" si="14"/>
+        <v>149.1140831579049</v>
+      </c>
+    </row>
+    <row r="299" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A299" s="10">
         <v>2.5833333330000001</v>
       </c>
-      <c r="B299">
+      <c r="B299" s="10">
         <v>249.07</v>
       </c>
-      <c r="C299" t="s">
+      <c r="C299" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A300">
+      <c r="H299" s="10">
+        <f t="shared" si="16"/>
+        <v>761.48</v>
+      </c>
+      <c r="I299" s="10">
+        <f t="shared" si="13"/>
+        <v>956.43000000000006</v>
+      </c>
+      <c r="J299" s="10">
+        <f>A302-A301</f>
+        <v>0.30000000000000027</v>
+      </c>
+      <c r="K299" s="10">
+        <f t="shared" si="14"/>
+        <v>286.92900000000026</v>
+      </c>
+    </row>
+    <row r="300" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A300" s="10">
         <v>2.8666666670000001</v>
       </c>
-      <c r="B300">
+      <c r="B300" s="10">
         <v>270.69</v>
       </c>
-      <c r="C300" t="s">
+      <c r="C300" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A301">
+      <c r="H300" s="10">
+        <f>B302+20.4</f>
+        <v>1151.3800000000001</v>
+      </c>
+      <c r="I300" s="10">
+        <f t="shared" si="13"/>
+        <v>1334.9950000000001</v>
+      </c>
+      <c r="J300" s="10">
+        <f>A303-A302</f>
+        <v>0.28333333299999985</v>
+      </c>
+      <c r="K300" s="10">
+        <f t="shared" si="14"/>
+        <v>378.24858288833485</v>
+      </c>
+    </row>
+    <row r="301" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A301" s="10">
         <v>3.15</v>
       </c>
-      <c r="B301">
+      <c r="B301" s="10">
         <v>741.08</v>
       </c>
-      <c r="C301" t="s">
+      <c r="C301" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A302">
+      <c r="H301" s="10">
+        <f t="shared" ref="H301:H303" si="17">B303+20.4</f>
+        <v>1518.6100000000001</v>
+      </c>
+      <c r="I301" s="10">
+        <f t="shared" si="13"/>
+        <v>1506.38</v>
+      </c>
+      <c r="J301" s="10">
+        <f>A304-A303</f>
+        <v>0.29999999999999982</v>
+      </c>
+      <c r="K301" s="10">
+        <f t="shared" si="14"/>
+        <v>451.91399999999976</v>
+      </c>
+    </row>
+    <row r="302" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A302" s="10">
         <v>3.45</v>
       </c>
-      <c r="B302">
+      <c r="B302" s="10">
         <v>1130.98</v>
       </c>
-      <c r="C302" t="s">
+      <c r="C302" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A303">
+      <c r="E302" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F302" s="9"/>
+      <c r="G302">
+        <v>4.0666700000000002</v>
+      </c>
+      <c r="H302" s="10">
+        <f t="shared" si="17"/>
+        <v>1494.15</v>
+      </c>
+      <c r="I302" s="10">
+        <f>(H303+H302)/2</f>
+        <v>1511.6000000000001</v>
+      </c>
+      <c r="J302" s="10">
+        <f>G302-A304</f>
+        <v>3.3336667000000375E-2</v>
+      </c>
+      <c r="K302" s="10">
+        <f t="shared" si="14"/>
+        <v>50.391705837200568</v>
+      </c>
+    </row>
+    <row r="303" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A303" s="10">
         <v>3.733333333</v>
       </c>
-      <c r="B303">
+      <c r="B303" s="10">
         <v>1498.21</v>
       </c>
-      <c r="C303" t="s">
+      <c r="C303" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A304">
+      <c r="H303" s="10">
+        <f>B305+20.4</f>
+        <v>1529.0500000000002</v>
+      </c>
+      <c r="K303" s="10">
+        <f>SUM(K291:K302)</f>
+        <v>2132.9967886409754</v>
+      </c>
+    </row>
+    <row r="304" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A304" s="10">
         <v>4.0333333329999999</v>
       </c>
-      <c r="B304">
+      <c r="B304" s="10">
         <v>1473.75</v>
       </c>
-      <c r="C304" t="s">
+      <c r="C304" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A305">
+    <row r="305" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A305" s="10">
         <v>4.3166666669999998</v>
       </c>
-      <c r="B305">
+      <c r="B305" s="10">
         <v>1508.65</v>
       </c>
-      <c r="C305" t="s">
+      <c r="C305" s="10" t="s">
         <v>22</v>
       </c>
     </row>
@@ -4858,7 +5722,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>0.35</v>
       </c>
@@ -4869,7 +5733,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>0.61666666699999995</v>
       </c>
@@ -4880,7 +5744,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>0.95</v>
       </c>
@@ -4891,7 +5755,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>1.266666667</v>
       </c>
@@ -4902,7 +5766,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>1.55</v>
       </c>
@@ -4913,7 +5777,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="342" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>1.85</v>
       </c>
@@ -4924,7 +5788,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>2.1166666670000001</v>
       </c>
@@ -4935,7 +5799,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>2.4166666669999999</v>
       </c>
@@ -4946,7 +5810,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="345" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>2.6833333330000002</v>
       </c>
@@ -4957,7 +5821,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>2.9666666670000001</v>
       </c>
@@ -4968,7 +5832,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>3.25</v>
       </c>
@@ -4979,7 +5843,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>3.516666667</v>
       </c>
@@ -4990,7 +5854,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A349">
         <v>3.8166666669999998</v>
       </c>
@@ -5001,7 +5865,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A350">
         <v>4.1166666669999996</v>
       </c>
@@ -5012,7 +5876,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>4.4000000000000004</v>
       </c>
@@ -5022,283 +5886,680 @@
       <c r="C351" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A352">
+      <c r="H351" t="s">
+        <v>59</v>
+      </c>
+      <c r="I351" t="s">
+        <v>60</v>
+      </c>
+      <c r="J351" t="s">
+        <v>61</v>
+      </c>
+      <c r="K351" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="352" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A352" s="10">
         <v>0</v>
       </c>
-      <c r="B352">
+      <c r="B352" s="10">
         <v>-19.09</v>
       </c>
-      <c r="C352" t="s">
+      <c r="C352" s="10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A353">
+      <c r="H352" s="10">
+        <f>B352+19.09</f>
+        <v>0</v>
+      </c>
+      <c r="I352" s="10">
+        <f>(H353+H352)/2</f>
+        <v>45.005000000000003</v>
+      </c>
+      <c r="J352" s="10">
+        <f>A353-A352</f>
         <v>0.15</v>
       </c>
-      <c r="B353">
+      <c r="K352" s="10">
+        <f>J352*I352</f>
+        <v>6.75075</v>
+      </c>
+    </row>
+    <row r="353" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A353" s="10">
+        <v>0.15</v>
+      </c>
+      <c r="B353" s="10">
         <v>70.92</v>
       </c>
-      <c r="C353" t="s">
+      <c r="C353" s="10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A354">
+      <c r="H353" s="10">
+        <f t="shared" ref="H353:H364" si="18">B353+19.09</f>
+        <v>90.01</v>
+      </c>
+      <c r="I353" s="10">
+        <f t="shared" ref="I353:I364" si="19">(H354+H353)/2</f>
+        <v>230.82999999999998</v>
+      </c>
+      <c r="J353" s="10">
+        <f t="shared" ref="J353:J363" si="20">A354-A353</f>
+        <v>0.71666666699999992</v>
+      </c>
+      <c r="K353" s="10">
+        <f t="shared" ref="K353:K363" si="21">J353*I353</f>
+        <v>165.42816674360998</v>
+      </c>
+    </row>
+    <row r="354" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A354" s="10">
         <v>0.86666666699999995</v>
       </c>
-      <c r="B354">
+      <c r="B354" s="10">
         <v>352.56</v>
       </c>
-      <c r="C354" t="s">
+      <c r="C354" s="10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A355">
+      <c r="H354" s="10">
+        <f t="shared" si="18"/>
+        <v>371.65</v>
+      </c>
+      <c r="I354" s="10">
+        <f t="shared" si="19"/>
+        <v>382.43999999999994</v>
+      </c>
+      <c r="J354" s="10">
+        <f t="shared" si="20"/>
+        <v>0.31666666600000004</v>
+      </c>
+      <c r="K354" s="10">
+        <f t="shared" si="21"/>
+        <v>121.10599974503999</v>
+      </c>
+    </row>
+    <row r="355" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A355" s="10">
         <v>1.183333333</v>
       </c>
-      <c r="B355">
+      <c r="B355" s="10">
         <v>374.14</v>
       </c>
-      <c r="C355" t="s">
+      <c r="C355" s="10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A356">
+      <c r="H355" s="10">
+        <f t="shared" si="18"/>
+        <v>393.22999999999996</v>
+      </c>
+      <c r="I355" s="10">
+        <f t="shared" si="19"/>
+        <v>381.18999999999994</v>
+      </c>
+      <c r="J355" s="10">
+        <f t="shared" si="20"/>
+        <v>0.4166666670000001</v>
+      </c>
+      <c r="K355" s="10">
+        <f t="shared" si="21"/>
+        <v>158.82916679373002</v>
+      </c>
+    </row>
+    <row r="356" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A356" s="10">
         <v>1.6</v>
       </c>
-      <c r="B356">
+      <c r="B356" s="10">
         <v>350.06</v>
       </c>
-      <c r="C356" t="s">
+      <c r="C356" s="10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="357" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A357">
+      <c r="H356" s="10">
+        <f t="shared" si="18"/>
+        <v>369.15</v>
+      </c>
+      <c r="I356" s="10">
+        <f t="shared" si="19"/>
+        <v>370.21499999999997</v>
+      </c>
+      <c r="J356" s="10">
+        <f t="shared" si="20"/>
+        <v>0.31666666700000001</v>
+      </c>
+      <c r="K356" s="10">
+        <f t="shared" si="21"/>
+        <v>117.23475012340499</v>
+      </c>
+    </row>
+    <row r="357" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A357" s="10">
         <v>1.9166666670000001</v>
       </c>
-      <c r="B357">
+      <c r="B357" s="10">
         <v>352.19</v>
       </c>
-      <c r="C357" t="s">
+      <c r="C357" s="10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="358" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A358">
+      <c r="H357" s="10">
+        <f t="shared" si="18"/>
+        <v>371.28</v>
+      </c>
+      <c r="I357" s="10">
+        <f t="shared" si="19"/>
+        <v>370.93499999999995</v>
+      </c>
+      <c r="J357" s="10">
+        <f t="shared" si="20"/>
+        <v>0.39999999999999969</v>
+      </c>
+      <c r="K357" s="10">
+        <f t="shared" si="21"/>
+        <v>148.37399999999985</v>
+      </c>
+    </row>
+    <row r="358" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A358" s="10">
         <v>2.3166666669999998</v>
       </c>
-      <c r="B358">
+      <c r="B358" s="10">
         <v>351.5</v>
       </c>
-      <c r="C358" t="s">
+      <c r="C358" s="10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="359" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A359">
+      <c r="H358" s="10">
+        <f t="shared" si="18"/>
+        <v>370.59</v>
+      </c>
+      <c r="I358" s="10">
+        <f t="shared" si="19"/>
+        <v>375.80499999999995</v>
+      </c>
+      <c r="J358" s="10">
+        <f t="shared" si="20"/>
+        <v>0.38333333300000039</v>
+      </c>
+      <c r="K358" s="10">
+        <f t="shared" si="21"/>
+        <v>144.05858320806513</v>
+      </c>
+    </row>
+    <row r="359" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A359" s="10">
         <v>2.7</v>
       </c>
-      <c r="B359">
+      <c r="B359" s="10">
         <v>361.93</v>
       </c>
-      <c r="C359" t="s">
+      <c r="C359" s="10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="360" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A360">
+      <c r="H359" s="10">
+        <f t="shared" si="18"/>
+        <v>381.02</v>
+      </c>
+      <c r="I359" s="10">
+        <f t="shared" si="19"/>
+        <v>419.11500000000001</v>
+      </c>
+      <c r="J359" s="10">
+        <f>A360-A359</f>
+        <v>0.36666666699999961</v>
+      </c>
+      <c r="K359" s="10">
+        <f t="shared" si="21"/>
+        <v>153.67550013970484</v>
+      </c>
+    </row>
+    <row r="360" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A360" s="10">
         <v>3.0666666669999998</v>
       </c>
-      <c r="B360">
+      <c r="B360" s="10">
         <v>438.12</v>
       </c>
-      <c r="C360" t="s">
+      <c r="C360" s="10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="361" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A361">
+      <c r="H360" s="10">
+        <f t="shared" si="18"/>
+        <v>457.21</v>
+      </c>
+      <c r="I360" s="10">
+        <f t="shared" si="19"/>
+        <v>714.32</v>
+      </c>
+      <c r="J360" s="10">
+        <f>A361-A360</f>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="K360" s="10">
+        <f t="shared" si="21"/>
+        <v>250.01200000000009</v>
+      </c>
+    </row>
+    <row r="361" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A361" s="10">
         <v>3.4166666669999999</v>
       </c>
-      <c r="B361">
+      <c r="B361" s="10">
         <v>952.34</v>
       </c>
-      <c r="C361" t="s">
+      <c r="C361" s="10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="362" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A362">
+      <c r="H361" s="10">
+        <f t="shared" si="18"/>
+        <v>971.43000000000006</v>
+      </c>
+      <c r="I361" s="10">
+        <f t="shared" si="19"/>
+        <v>1007.14</v>
+      </c>
+      <c r="J361" s="10">
+        <f>A362-A361</f>
+        <v>0.31666666600000015</v>
+      </c>
+      <c r="K361" s="10">
+        <f t="shared" si="21"/>
+        <v>318.92766599524015</v>
+      </c>
+    </row>
+    <row r="362" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A362" s="10">
         <v>3.733333333</v>
       </c>
-      <c r="B362">
+      <c r="B362" s="10">
         <v>1023.76</v>
       </c>
-      <c r="C362" t="s">
+      <c r="C362" s="10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="363" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A363">
+      <c r="E362" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F362" s="9"/>
+      <c r="G362">
+        <v>4.0666700000000002</v>
+      </c>
+      <c r="H362" s="10">
+        <f t="shared" si="18"/>
+        <v>1042.8499999999999</v>
+      </c>
+      <c r="I362" s="10">
+        <f t="shared" si="19"/>
+        <v>1376.7749999999999</v>
+      </c>
+      <c r="J362" s="10">
+        <f>G362-A362</f>
+        <v>0.3333366670000002</v>
+      </c>
+      <c r="K362" s="10">
+        <f t="shared" si="21"/>
+        <v>458.92958970892522</v>
+      </c>
+    </row>
+    <row r="363" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A363" s="10">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B363">
+      <c r="B363" s="10">
         <v>1691.61</v>
       </c>
-      <c r="C363" t="s">
+      <c r="C363" s="10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="364" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A364">
+      <c r="H363" s="10">
+        <f t="shared" si="18"/>
+        <v>1710.6999999999998</v>
+      </c>
+      <c r="I363" s="10">
+        <f t="shared" si="19"/>
+        <v>1816.915</v>
+      </c>
+      <c r="J363" s="10">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="K363" s="10">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="364" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A364" s="10">
         <v>4.5</v>
       </c>
-      <c r="B364">
+      <c r="B364" s="10">
         <v>1904.04</v>
       </c>
-      <c r="C364" t="s">
+      <c r="C364" s="10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="365" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A365">
+      <c r="H364" s="10">
+        <f t="shared" si="18"/>
+        <v>1923.1299999999999</v>
+      </c>
+      <c r="K364" s="10">
+        <f>SUM(K352:K363)</f>
+        <v>2043.3261724577203</v>
+      </c>
+    </row>
+    <row r="365" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A365" s="9">
         <v>0</v>
       </c>
-      <c r="B365">
+      <c r="B365" s="9">
         <v>-22.72</v>
       </c>
-      <c r="C365" t="s">
+      <c r="C365" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="366" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A366">
+    <row r="366" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A366" s="9">
         <v>0.233333333</v>
       </c>
-      <c r="B366">
+      <c r="B366" s="9">
         <v>20.97</v>
       </c>
-      <c r="C366" t="s">
+      <c r="C366" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="367" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A367">
+      <c r="H366" t="s">
+        <v>59</v>
+      </c>
+      <c r="I366" t="s">
+        <v>60</v>
+      </c>
+      <c r="J366" t="s">
+        <v>61</v>
+      </c>
+      <c r="K366" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="367" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A367" s="9">
         <v>0.61666666699999995</v>
       </c>
-      <c r="B367">
+      <c r="B367" s="9">
         <v>305.01</v>
       </c>
-      <c r="C367" t="s">
+      <c r="C367" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="368" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A368">
+      <c r="H367" s="9">
+        <f>B365+22.72</f>
+        <v>0</v>
+      </c>
+      <c r="I367" s="9">
+        <f>(H368+H367)/2</f>
+        <v>21.844999999999999</v>
+      </c>
+      <c r="J367" s="9">
+        <f>A366-A365</f>
+        <v>0.233333333</v>
+      </c>
+      <c r="K367" s="9">
+        <f>I367*J367</f>
+        <v>5.0971666593849996</v>
+      </c>
+    </row>
+    <row r="368" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A368" s="9">
         <v>1.066666667</v>
       </c>
-      <c r="B368">
+      <c r="B368" s="9">
         <v>346.8</v>
       </c>
-      <c r="C368" t="s">
+      <c r="C368" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="369" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A369">
+      <c r="H368" s="9">
+        <f t="shared" ref="H368:H378" si="22">B366+22.72</f>
+        <v>43.69</v>
+      </c>
+      <c r="I368" s="9">
+        <f t="shared" ref="I368:I377" si="23">(H369+H368)/2</f>
+        <v>185.71</v>
+      </c>
+      <c r="J368" s="9">
+        <f t="shared" ref="J368:J377" si="24">A367-A366</f>
+        <v>0.38333333399999991</v>
+      </c>
+      <c r="K368" s="9">
+        <f t="shared" ref="K368:K377" si="25">I368*J368</f>
+        <v>71.188833457139992</v>
+      </c>
+    </row>
+    <row r="369" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A369" s="9">
         <v>1.55</v>
       </c>
-      <c r="B369">
+      <c r="B369" s="9">
         <v>323.73</v>
       </c>
-      <c r="C369" t="s">
+      <c r="C369" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="370" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A370">
+      <c r="H369" s="9">
+        <f t="shared" si="22"/>
+        <v>327.73</v>
+      </c>
+      <c r="I369" s="9">
+        <f t="shared" si="23"/>
+        <v>348.625</v>
+      </c>
+      <c r="J369" s="9">
+        <f t="shared" si="24"/>
+        <v>0.45000000000000007</v>
+      </c>
+      <c r="K369" s="9">
+        <f t="shared" si="25"/>
+        <v>156.88125000000002</v>
+      </c>
+    </row>
+    <row r="370" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A370" s="9">
         <v>1.9666666669999999</v>
       </c>
-      <c r="B370">
+      <c r="B370" s="9">
         <v>380.81</v>
       </c>
-      <c r="C370" t="s">
+      <c r="C370" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="371" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A371">
+      <c r="H370" s="9">
+        <f t="shared" si="22"/>
+        <v>369.52</v>
+      </c>
+      <c r="I370" s="9">
+        <f t="shared" si="23"/>
+        <v>357.98500000000001</v>
+      </c>
+      <c r="J370" s="9">
+        <f t="shared" si="24"/>
+        <v>0.48333333300000003</v>
+      </c>
+      <c r="K370" s="9">
+        <f t="shared" si="25"/>
+        <v>173.02608321400501</v>
+      </c>
+    </row>
+    <row r="371" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A371" s="9">
         <v>2.4</v>
       </c>
-      <c r="B371">
+      <c r="B371" s="9">
         <v>995.51</v>
       </c>
-      <c r="C371" t="s">
+      <c r="C371" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="372" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A372">
+      <c r="H371" s="9">
+        <f t="shared" si="22"/>
+        <v>346.45000000000005</v>
+      </c>
+      <c r="I371" s="9">
+        <f t="shared" si="23"/>
+        <v>374.99</v>
+      </c>
+      <c r="J371" s="9">
+        <f t="shared" si="24"/>
+        <v>0.41666666699999988</v>
+      </c>
+      <c r="K371" s="9">
+        <f t="shared" si="25"/>
+        <v>156.24583345832997</v>
+      </c>
+    </row>
+    <row r="372" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A372" s="9">
         <v>2.7833333329999999</v>
       </c>
-      <c r="B372">
+      <c r="B372" s="9">
         <v>1713.79</v>
       </c>
-      <c r="C372" t="s">
+      <c r="C372" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="373" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A373">
+      <c r="H372" s="9">
+        <f t="shared" si="22"/>
+        <v>403.53</v>
+      </c>
+      <c r="I372" s="9">
+        <f t="shared" si="23"/>
+        <v>710.88</v>
+      </c>
+      <c r="J372" s="9">
+        <f t="shared" si="24"/>
+        <v>0.43333333299999999</v>
+      </c>
+      <c r="K372" s="9">
+        <f t="shared" si="25"/>
+        <v>308.04799976303997</v>
+      </c>
+    </row>
+    <row r="373" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A373" s="9">
         <v>3.2833333329999999</v>
       </c>
-      <c r="B373">
+      <c r="B373" s="9">
         <v>1805.2</v>
       </c>
-      <c r="C373" t="s">
+      <c r="C373" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="374" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A374">
+      <c r="H373" s="9">
+        <f t="shared" si="22"/>
+        <v>1018.23</v>
+      </c>
+      <c r="I373" s="9">
+        <f t="shared" si="23"/>
+        <v>1377.37</v>
+      </c>
+      <c r="J373" s="9">
+        <f t="shared" si="24"/>
+        <v>0.38333333299999994</v>
+      </c>
+      <c r="K373" s="9">
+        <f t="shared" si="25"/>
+        <v>527.99183287420988</v>
+      </c>
+    </row>
+    <row r="374" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A374" s="9">
         <v>3.7</v>
       </c>
-      <c r="B374">
+      <c r="B374" s="9">
         <v>1968.83</v>
       </c>
-      <c r="C374" t="s">
+      <c r="C374" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="375" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A375">
+      <c r="E374" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G374">
+        <v>4.0666700000000002</v>
+      </c>
+      <c r="H374" s="9">
+        <f t="shared" si="22"/>
+        <v>1736.51</v>
+      </c>
+      <c r="I374" s="9">
+        <f t="shared" si="23"/>
+        <v>1782.2150000000001</v>
+      </c>
+      <c r="J374" s="9">
+        <f>A373-A372</f>
+        <v>0.5</v>
+      </c>
+      <c r="K374" s="9">
+        <f t="shared" si="25"/>
+        <v>891.10750000000007</v>
+      </c>
+    </row>
+    <row r="375" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A375" s="9">
         <v>4.3499999999999996</v>
       </c>
-      <c r="B375">
+      <c r="B375" s="9">
         <v>2145.4499999999998</v>
       </c>
-      <c r="C375" t="s">
+      <c r="C375" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="376" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A376">
+      <c r="H375" s="9">
+        <f t="shared" si="22"/>
+        <v>1827.92</v>
+      </c>
+      <c r="I375" s="9">
+        <f t="shared" si="23"/>
+        <v>1909.7350000000001</v>
+      </c>
+      <c r="J375" s="9">
+        <f>A374-A373</f>
+        <v>0.41666666700000032</v>
+      </c>
+      <c r="K375" s="9">
+        <f t="shared" si="25"/>
+        <v>795.72291730324571</v>
+      </c>
+    </row>
+    <row r="376" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A376" s="9">
         <v>4.4666666670000001</v>
       </c>
-      <c r="B376">
+      <c r="B376" s="9">
         <v>1962.59</v>
       </c>
-      <c r="C376" t="s">
+      <c r="C376" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="377" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H376" s="9">
+        <f t="shared" si="22"/>
+        <v>1991.55</v>
+      </c>
+      <c r="I376" s="9">
+        <f t="shared" si="23"/>
+        <v>2079.8599999999997</v>
+      </c>
+      <c r="J376" s="9">
+        <f>G374-A374</f>
+        <v>0.36667000000000005</v>
+      </c>
+      <c r="K376" s="9">
+        <f t="shared" si="25"/>
+        <v>762.62226620000001</v>
+      </c>
+    </row>
+    <row r="377" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A377">
         <v>0</v>
       </c>
@@ -5308,8 +6569,23 @@
       <c r="C377" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="378" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H377" s="9">
+        <f t="shared" si="22"/>
+        <v>2168.1699999999996</v>
+      </c>
+      <c r="I377" s="9">
+        <f t="shared" si="23"/>
+        <v>2076.7399999999998</v>
+      </c>
+      <c r="J377" s="9">
+        <v>0</v>
+      </c>
+      <c r="K377" s="9">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="378" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A378">
         <v>0.18333333299999999</v>
       </c>
@@ -5319,8 +6595,16 @@
       <c r="C378" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="379" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H378" s="9">
+        <f>B376+22.72</f>
+        <v>1985.31</v>
+      </c>
+      <c r="K378" s="9">
+        <f>SUM(K367:K377)</f>
+        <v>3847.9316829293557</v>
+      </c>
+    </row>
+    <row r="379" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A379">
         <v>0.5</v>
       </c>
@@ -5331,7 +6615,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="380" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A380">
         <v>0.8</v>
       </c>
@@ -5342,7 +6626,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="381" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A381">
         <v>1.1333333329999999</v>
       </c>
@@ -5353,7 +6637,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="382" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A382">
         <v>1.4666666669999999</v>
       </c>
@@ -5364,7 +6648,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="383" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A383">
         <v>1.9166666670000001</v>
       </c>
@@ -5375,7 +6659,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="384" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A384">
         <v>2.25</v>
       </c>

</xml_diff>